<commit_message>
working on sec IV: refining intro and BJ section
git-svn-id: file://localhost/tmp/svn2git/svn@5405 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/new_results_al.xlsx
+++ b/papers/troy/pstar/perf/new_results_al.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
     <t>wu-runtime avg</t>
   </si>
@@ -110,6 +110,14 @@
   </si>
   <si>
     <t>TROY/PJ Framework Startup</t>
+  </si>
+  <si>
+    <t>TROY-BJ
+(Globus)</t>
+  </si>
+  <si>
+    <t>TROY-BJ
+(CONDOR)</t>
   </si>
 </sst>
 </file>
@@ -621,9 +629,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.124830116700806"/>
-          <c:y val="0.0362544583112882"/>
+          <c:y val="0.0743756264639827"/>
           <c:w val="0.832387491197747"/>
-          <c:h val="0.864467710310915"/>
+          <c:h val="0.826346488853631"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -659,13 +667,13 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>TROY-BJ</c:v>
+                  <c:v>TROY-BJ_x000d_(Globus)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>TROY-DIANE</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>TROY-CONDOR</c:v>
+                  <c:v>TROY-BJ_x000d_(CONDOR)</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>TROY-BJ_x000d_TROY-DIANE</c:v>
@@ -723,13 +731,13 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>TROY-BJ</c:v>
+                  <c:v>TROY-BJ_x000d_(Globus)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>TROY-DIANE</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>TROY-CONDOR</c:v>
+                  <c:v>TROY-BJ_x000d_(CONDOR)</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>TROY-BJ_x000d_TROY-DIANE</c:v>
@@ -787,13 +795,13 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>TROY-BJ</c:v>
+                  <c:v>TROY-BJ_x000d_(Globus)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>TROY-DIANE</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>TROY-CONDOR</c:v>
+                  <c:v>TROY-BJ_x000d_(CONDOR)</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>TROY-BJ_x000d_TROY-DIANE</c:v>
@@ -833,11 +841,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="622202472"/>
-        <c:axId val="874999128"/>
+        <c:axId val="607735304"/>
+        <c:axId val="607745112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="622202472"/>
+        <c:axId val="607735304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -851,7 +859,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000">
+              <a:defRPr sz="2400" b="1">
                 <a:latin typeface="Helvetica"/>
                 <a:cs typeface="Helvetica"/>
               </a:defRPr>
@@ -859,7 +867,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="874999128"/>
+        <c:crossAx val="607745112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -867,7 +875,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="874999128"/>
+        <c:axId val="607745112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,7 +944,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="622202472"/>
+        <c:crossAx val="607735304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -953,8 +961,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.488530058444365"/>
-          <c:y val="0.0217836279898975"/>
+          <c:x val="0.494496645556537"/>
+          <c:y val="0.0396851513759926"/>
           <c:w val="0.502700092082762"/>
           <c:h val="0.185279690982023"/>
         </c:manualLayout>
@@ -1006,14 +1014,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>97</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1360,8 +1368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA56" sqref="AA56"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="Y75" sqref="Y75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1372,8 +1380,8 @@
     <col min="4" max="4" width="24.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17" customHeight="1"/>
-    <row r="7" spans="1:14">
+    <row r="1" spans="1:15" ht="17" customHeight="1"/>
+    <row r="7" spans="1:15">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -1381,7 +1389,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="39" thickBot="1">
+    <row r="8" spans="1:15" ht="39" thickBot="1">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1410,7 +1418,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" thickTop="1">
+    <row r="9" spans="1:15" ht="16" thickTop="1">
       <c r="C9">
         <v>81.040000000000006</v>
       </c>
@@ -1433,7 +1441,7 @@
         <v>81.900000000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="C10">
         <v>75.709999999999994</v>
       </c>
@@ -1456,7 +1464,7 @@
         <v>87.53</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="C11">
         <v>65.099999999999994</v>
       </c>
@@ -1479,7 +1487,7 @@
         <v>87.6</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="J12">
         <f>AVERAGE(J9:J11)</f>
         <v>83.850000000000009</v>
@@ -1500,8 +1508,12 @@
         <f>AVERAGE(J12:M12)</f>
         <v>84.763333333333335</v>
       </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="O12">
+        <f>N12/N30</f>
+        <v>1.6411100354953212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="C13">
         <f>AVERAGE(C9:C11)</f>
         <v>73.95</v>
@@ -1515,7 +1527,7 @@
         <v>166.79666666666665</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="14" customHeight="1"/>
+    <row r="15" spans="1:15" ht="14" customHeight="1"/>
     <row r="20" spans="1:15" ht="39" thickBot="1">
       <c r="A20" s="2" t="s">
         <v>2</v>
@@ -1713,6 +1725,14 @@
       <c r="M30">
         <v>51.65</v>
       </c>
+      <c r="N30">
+        <f>AVERAGE(J30:M30)</f>
+        <v>51.65</v>
+      </c>
+      <c r="O30">
+        <f>N30/N12</f>
+        <v>0.60934366274725704</v>
+      </c>
     </row>
     <row r="31" spans="1:15">
       <c r="C31">
@@ -2045,9 +2065,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
-      <c r="A69" t="s">
-        <v>1</v>
+    <row r="69" spans="1:5" ht="30">
+      <c r="A69" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="B69">
         <v>73.95</v>
@@ -2079,9 +2099,9 @@
         <v>240.47</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
-      <c r="A71" t="s">
-        <v>22</v>
+    <row r="71" spans="1:5" ht="30">
+      <c r="A71" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="B71">
         <v>37.299999999999997</v>

</xml_diff>

<commit_message>
pending commits, updated rebuttle file
git-svn-id: file://localhost/tmp/svn2git/svn@5776 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/new_results_al.xlsx
+++ b/papers/troy/pstar/perf/new_results_al.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
   <si>
     <t>wu-runtime avg</t>
   </si>
@@ -118,6 +118,9 @@
   <si>
     <t>TROY-BJ
 (Condor)</t>
+  </si>
+  <si>
+    <t>BFAST Runtime</t>
   </si>
 </sst>
 </file>
@@ -712,7 +715,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>BFAST-Runtime</c:v>
+                  <c:v>BFAST Runtime</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1370,7 +1373,7 @@
   <dimension ref="A1:O72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="Y83" sqref="Y83"/>
+      <selection activeCell="O49" sqref="O49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2057,7 +2060,7 @@
         <v>29</v>
       </c>
       <c r="C68" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D68" t="s">
         <v>26</v>

</xml_diff>